<commit_message>
Fix some bug and update the RoC curve classifier name
</commit_message>
<xml_diff>
--- a/Result/MIFSBasedResult.xlsx
+++ b/Result/MIFSBasedResult.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,28 +471,28 @@
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7400881057268722</v>
+        <v>0.73568281938326</v>
       </c>
       <c r="D2" t="n">
-        <v>0.739869585468095</v>
+        <v>0.7354836205558143</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7394204328642848</v>
+        <v>0.7351172480739726</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7398695531981481</v>
+        <v>0.7354835935802485</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7400881057268722</v>
+        <v>0.73568281938326</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7396510652093178</v>
+        <v>0.7352844217283686</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2603489347906822</v>
+        <v>0.2647155782716314</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2599118942731278</v>
+        <v>0.26431718061674</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -695,28 +695,28 @@
         <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7533039647577092</v>
+        <v>0.73568281938326</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7530662940537184</v>
+        <v>0.7352895513119081</v>
       </c>
       <c r="E9" t="n">
-        <v>0.7525546543702912</v>
+        <v>0.7335098391166802</v>
       </c>
       <c r="F9" t="n">
-        <v>0.7530662565488098</v>
+        <v>0.7352894461425998</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7533039647577092</v>
+        <v>0.73568281938326</v>
       </c>
       <c r="H9" t="n">
-        <v>0.7528286233497274</v>
+        <v>0.7348962832405563</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2471713766502726</v>
+        <v>0.2651037167594437</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2466960352422908</v>
+        <v>0.26431718061674</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -724,28 +724,28 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="n">
         <v>0.7533039647577092</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7530662940537184</v>
+        <v>0.7531439217512809</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7525546543702912</v>
+        <v>0.7529587207338903</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7530662565488098</v>
+        <v>0.7531439047467194</v>
       </c>
       <c r="G10" t="n">
         <v>0.7533039647577092</v>
       </c>
       <c r="H10" t="n">
-        <v>0.7528286233497274</v>
+        <v>0.7529838787448525</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2471713766502726</v>
+        <v>0.2470161212551475</v>
       </c>
       <c r="J10" t="n">
         <v>0.2466960352422908</v>
@@ -756,31 +756,31 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7533039647577092</v>
+        <v>0.7224669603524229</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7531439217512809</v>
+        <v>0.7222869119701909</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7529587207338903</v>
+        <v>0.7219812815803627</v>
       </c>
       <c r="F11" t="n">
-        <v>0.7531439047467194</v>
+        <v>0.7222868895293715</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7533039647577092</v>
+        <v>0.7224669603524229</v>
       </c>
       <c r="H11" t="n">
-        <v>0.7529838787448525</v>
+        <v>0.7221068635879591</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2470161212551475</v>
+        <v>0.2778931364120409</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2466960352422908</v>
+        <v>0.2775330396475771</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -788,31 +788,31 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7268722466960352</v>
+        <v>0.7224669603524229</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7267116907312529</v>
+        <v>0.722442167365316</v>
       </c>
       <c r="E12" t="n">
-        <v>0.7264900122410928</v>
+        <v>0.7224561875997922</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7267116729950458</v>
+        <v>0.7224421669398894</v>
       </c>
       <c r="G12" t="n">
-        <v>0.7268722466960352</v>
+        <v>0.7224669603524229</v>
       </c>
       <c r="H12" t="n">
-        <v>0.7265511347664706</v>
+        <v>0.7224173743782091</v>
       </c>
       <c r="I12" t="n">
-        <v>0.2734488652335294</v>
+        <v>0.2775826256217909</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2731277533039648</v>
+        <v>0.2775330396475771</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -820,63 +820,31 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7224669603524229</v>
+        <v>0.4933920704845815</v>
       </c>
       <c r="D13" t="n">
-        <v>0.722442167365316</v>
+        <v>0.493828598043782</v>
       </c>
       <c r="E13" t="n">
-        <v>0.7224561875997922</v>
+        <v>0.4883701562454827</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7224421669398894</v>
+        <v>0.4938284051060422</v>
       </c>
       <c r="G13" t="n">
-        <v>0.7224669603524229</v>
+        <v>0.4933920704845815</v>
       </c>
       <c r="H13" t="n">
-        <v>0.7224173743782091</v>
+        <v>0.4942651256029826</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2775826256217909</v>
+        <v>0.5057348743970174</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2775330396475771</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.4889867841409692</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.4894038192827201</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.4843655794407093</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.489403641598838</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.4889867841409692</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.489820854424471</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.5101791455755289</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.5110132158590308</v>
+        <v>0.5066079295154184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>